<commit_message>
Enregistrement fonctionnelle + SpellAlchiDebut + NouvelleRace
</commit_message>
<xml_diff>
--- a/race.xlsx
+++ b/race.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" tabRatio="638"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="157">
   <si>
     <t>Race</t>
   </si>
@@ -130,15 +130,9 @@
     <t>Kitsune</t>
   </si>
   <si>
-    <t>Nagaji</t>
-  </si>
-  <si>
     <t>Samsaran</t>
   </si>
   <si>
-    <t>Strix</t>
-  </si>
-  <si>
     <t>Suli</t>
   </si>
   <si>
@@ -151,9 +145,6 @@
     <t>Vishkanya</t>
   </si>
   <si>
-    <t>Wayang</t>
-  </si>
-  <si>
     <t>Drakéide</t>
   </si>
   <si>
@@ -181,9 +172,6 @@
     <t>BonusCha</t>
   </si>
   <si>
-    <t>Les petits wayangs sont des créatures du plan de l’Ombre.Ils sont si sensibles à l’ombre que celle-ci imprègne même leur philosophie:ils croient qu’au moment de leur mort,ils s’en retournent simplement aux ténèbres.Le mystère de leur existence insondable leur accorde la capacité à guérir de l’énergie négative comme de l’énergie positive.</t>
-  </si>
-  <si>
     <t>Étrangement beaux à l’extérieur et venimeux à l’intérieur,les vishkanyas voient le monde à travers les fentes de leurs yeux de serpent.Ils possèdent la même grâce que le serpent et la capacité à se glisser facilement hors de l’étreinte de leurs ennemis.Les vishkanyas ont la réputation d’être séducteurs et manipulateurs.Ils peuvent se servir de leur salive ou de leur sang pour empoisonner leurs armes.</t>
   </si>
   <si>
@@ -196,15 +184,9 @@
     <t>Aussi appelés les suli-janns,ces humanoïdes sont les enfants des mortels et des janns.Ces êtres puissants et charismatiques manifestent leur capacité à maîtriser les puissances élémentaires à l’adolescence,ce qui leur permet de manipuler la terre,le feu,la glace ou l’électricité.Cette puissance élémentaire a également tendance à se refléter dans la personnalité du suli.</t>
   </si>
   <si>
-    <t>Race déclinante chassée par les humains qui voient en eux des diables ailés,les strix sont les sombres maîtres des cieux nocturnes.Leurs conflits territoriaux ont alimenté leur haine pour les humains.Du fait de ces querelles interminables,ces créatures de la nuit les attaquent souvent à vue.</t>
-  </si>
-  <si>
     <t>Serviteurs fantomatiques du karma,les samsarans sont des créatures qui se sont réincarnées des centaines,sinon des milliers de fois dans l’espoir d’atteindre la véritable illumination.Contrairement aux humains et aux autres races,ces humanoïdes se souviennent de l’essentiel de leurs vies passées.</t>
   </si>
   <si>
-    <t>D’après les légendes,les nagas auraient créé les nagajis pour en faire une race de serviteurs,et les nagajis vénèreraient leurs créateurs comme des dieux vivants.Du fait de leur nature reptilienne et de leurs curieuses manières,ces étranges créatures à écailles inspirent la peur et l’émerveillement chez tous ceux qui n’appartiennent pas à leur genre.Ils sont résistants aux poisons et aux effets magiques mentaux.</t>
-  </si>
-  <si>
     <t>Ces hommes-renards métamorphes partagent le même amour de l’espièglerie,de l’art et des douceurs de la vie.Ils peuvent apparaître comme de simples humains ainsi que sous leur véritable forme,des humanoïdes semblables à des renards.Les kitsune sont des créatures vives d’esprit,agiles et grégaires:pour cette raison,un grand nombre d’entre eux deviennent des aventuriers.</t>
   </si>
   <si>
@@ -220,9 +202,6 @@
     <t>Survivants d’une culture terrestre dont la patrie fut détruite,les aquatiques furent sauvés et transformés par les aboleths en une race amphibie.S’ils apparaissent presque humains de bien des manières,leurs yeux d’un mauve éclatant et leurs branchies les trahissent.Solitaires et suspicieux,les aquatiques savent que le jour viendra où les aboleths réclameront la dette qui leur est due.</t>
   </si>
   <si>
-    <t>Enfants des guenaudes et de leurs amants mortels,les dopplegangers sont abandonnées et élevées par des parents de substitution.Lorsqu’elles atteignent la puberté, les dopplegangers,toujours de sexe féminin,répondent toutes à un appel spirituel pour découvrir leurs véritables origines.Grandes et minces,les cheveux sombres et les yeux vairons,les dopplegangers sont étrangement séduisantes.</t>
-  </si>
-  <si>
     <t>Les ifrits sont une race qui descend des mortels et des étranges habitants du plan du Feu.Leurs caractéristiques physiques et leur personnalité trahissent souvent leurs origines flamboyantes:ils sont généralement nerveux,indépendants et impérieux.Souvent écartés des villes à cause de leur capacité à manipuler le feu,les ifrits font de puissants ensorceleurs du feu et des guerriers capables de manier les flammes comme nulle autre race.</t>
   </si>
   <si>
@@ -401,9 +380,6 @@
   </si>
   <si>
     <t>Commun,Vishkanyan</t>
-  </si>
-  <si>
-    <t>Commun,Wayang</t>
   </si>
   <si>
     <t>pret</t>
@@ -453,12 +429,118 @@
 de la terre.Les nains ont aussi tendance à s’isoler et à se replier sur leurs traditions,au point de sombrer
 parfois dans la xénophobie.</t>
   </si>
+  <si>
+    <t>Dragon</t>
+  </si>
+  <si>
+    <t>Mort-vivant</t>
+  </si>
+  <si>
+    <t>Harpy</t>
+  </si>
+  <si>
+    <t>Centaure</t>
+  </si>
+  <si>
+    <t>Change-forme</t>
+  </si>
+  <si>
+    <t>Norse</t>
+  </si>
+  <si>
+    <t>Démon</t>
+  </si>
+  <si>
+    <t>Satyre</t>
+  </si>
+  <si>
+    <t>Minotaure/Haultosaurus</t>
+  </si>
+  <si>
+    <t>Inccube/Succube</t>
+  </si>
+  <si>
+    <t>Flageleur mentaux</t>
+  </si>
+  <si>
+    <t>Clown</t>
+  </si>
+  <si>
+    <t>Vampire</t>
+  </si>
+  <si>
+    <t>Ent</t>
+  </si>
+  <si>
+    <t>Drider</t>
+  </si>
+  <si>
+    <t>Lamia</t>
+  </si>
+  <si>
+    <t>Oni</t>
+  </si>
+  <si>
+    <t>Alraune</t>
+  </si>
+  <si>
+    <t>Homonculus</t>
+  </si>
+  <si>
+    <t>Adlet</t>
+  </si>
+  <si>
+    <t>Demi-Orgre</t>
+  </si>
+  <si>
+    <t>Géant(Feu,Froid,Cendre,Jungle,Pierre,Colline,Nuage)</t>
+  </si>
+  <si>
+    <t>Troll</t>
+  </si>
+  <si>
+    <t>Troglodyte</t>
+  </si>
+  <si>
+    <t>Gobelour</t>
+  </si>
+  <si>
+    <t>Sorcewyrd</t>
+  </si>
+  <si>
+    <t>Trox</t>
+  </si>
+  <si>
+    <t>Changelin</t>
+  </si>
+  <si>
+    <t>Enfants des guenaudes et de leurs amants mortels,les changelins sont abandonnées et élevées par des parents de substitution.Lorsqu’elles atteignent la puberté, les changelins,toujours de sexe féminin,répondent toutes à un appel spirituel pour découvrir leurs véritables origines.Grandes et minces,les cheveux sombres et les yeux vairons,les changelins sont étrangement séduisantes.</t>
+  </si>
+  <si>
+    <t>Slime</t>
+  </si>
+  <si>
+    <t>ALL GOOD</t>
+  </si>
+  <si>
+    <t>GENDER RESTRIC</t>
+  </si>
+  <si>
+    <t>TAILLE RESTRIC</t>
+  </si>
+  <si>
+    <t>Adaro(homme requin)</t>
+  </si>
+  <si>
+    <t>TAILLE&amp;&amp;GENDER 
+RESTRIC</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -472,13 +554,58 @@
       <name val="Courier New"/>
       <family val="3"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9933FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -493,7 +620,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -518,6 +645,31 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -571,6 +723,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF9933FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -619,10 +776,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="B2:O40" tableType="xml" totalsRowShown="0" dataDxfId="14" connectionId="1">
-  <autoFilter ref="B2:O40"/>
-  <sortState ref="B3:N40">
-    <sortCondition descending="1" ref="C2:C40"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="B2:O67" tableType="xml" totalsRowShown="0" dataDxfId="14" connectionId="1">
+  <autoFilter ref="B2:O67"/>
+  <sortState ref="B3:N37">
+    <sortCondition descending="1" ref="C2:C37"/>
   </sortState>
   <tableColumns count="14">
     <tableColumn id="1" uniqueName="nom" name="Race" dataDxfId="13">
@@ -966,10 +1123,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Feuil1"/>
-  <dimension ref="B1:O40"/>
+  <dimension ref="A1:Q67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:O31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -977,71 +1134,73 @@
     <col min="1" max="1" width="5.85546875" customWidth="1"/>
     <col min="2" max="2" width="18.140625" customWidth="1"/>
     <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="229.28515625" customWidth="1"/>
+    <col min="4" max="4" width="152.5703125" customWidth="1"/>
     <col min="5" max="10" width="5.7109375" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" customWidth="1"/>
+    <col min="11" max="11" width="4.85546875" customWidth="1"/>
     <col min="12" max="12" width="4.28515625" customWidth="1"/>
-    <col min="13" max="13" width="36.85546875" customWidth="1"/>
+    <col min="13" max="13" width="36" customWidth="1"/>
     <col min="14" max="14" width="4.28515625" customWidth="1"/>
-    <col min="15" max="15" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.5703125" customWidth="1"/>
+    <col min="15" max="15" width="4.7109375" customWidth="1"/>
+    <col min="16" max="16" width="4.28515625" customWidth="1"/>
+    <col min="17" max="17" width="20.140625" customWidth="1"/>
     <col min="19" max="19" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="D2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" t="s">
         <v>40</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
         <v>41</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
         <v>42</v>
       </c>
-      <c r="G2" t="s">
+      <c r="J2" t="s">
         <v>43</v>
       </c>
-      <c r="H2" t="s">
-        <v>44</v>
-      </c>
-      <c r="I2" t="s">
-        <v>45</v>
-      </c>
-      <c r="J2" t="s">
-        <v>46</v>
-      </c>
       <c r="K2" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="L2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="M2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="N2" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="O2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="3" spans="2:15" ht="60" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="11"/>
       <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="E3" s="5">
         <v>0</v>
@@ -1062,28 +1221,32 @@
         <v>0</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="L3" s="4">
         <v>9</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="O3" s="1"/>
-    </row>
-    <row r="4" spans="2:15" ht="75" x14ac:dyDescent="0.25">
+      <c r="Q3" s="18" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="11"/>
       <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="E4" s="5">
         <v>0</v>
@@ -1104,28 +1267,32 @@
         <v>0</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="L4" s="4">
         <v>9</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="O4" s="1"/>
-    </row>
-    <row r="5" spans="2:15" ht="75" x14ac:dyDescent="0.25">
+      <c r="Q4" s="19" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" s="11"/>
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="E5" s="5">
         <v>0</v>
@@ -1146,28 +1313,32 @@
         <v>0</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="L5" s="4">
         <v>9</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="O5" s="1"/>
-    </row>
-    <row r="6" spans="2:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="Q5" s="20" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="11"/>
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="E6" s="5">
         <v>-2</v>
@@ -1188,28 +1359,32 @@
         <v>2</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="L6" s="4">
         <v>6</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="O6" s="1"/>
-    </row>
-    <row r="7" spans="2:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="Q6" s="21" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="11"/>
       <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="E7" s="5">
         <v>-2</v>
@@ -1230,28 +1405,29 @@
         <v>2</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="L7" s="4">
         <v>6</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="O7" s="1"/>
     </row>
-    <row r="8" spans="2:15" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="11"/>
       <c r="B8" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="E8" s="5">
         <v>0</v>
@@ -1272,28 +1448,29 @@
         <v>0</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="L8" s="4">
         <v>9</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="O8" s="1"/>
     </row>
-    <row r="9" spans="2:15" ht="75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="11"/>
       <c r="B9" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="E9" s="5">
         <v>0</v>
@@ -1314,28 +1491,29 @@
         <v>-2</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="L9" s="4">
         <v>6</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="O9" s="1"/>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="11"/>
       <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="E10" s="5">
         <v>0</v>
@@ -1360,22 +1538,23 @@
         <v>9</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="O10" s="1"/>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="14"/>
       <c r="B11" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E11" s="5">
         <v>0</v>
@@ -1400,22 +1579,23 @@
         <v>9</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="O11" s="1"/>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="11"/>
       <c r="B12" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E12" s="5">
         <v>0</v>
@@ -1440,22 +1620,23 @@
         <v>9</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="O12" s="1"/>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="12"/>
       <c r="B13" s="2" t="s">
-        <v>24</v>
+        <v>149</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>60</v>
+        <v>150</v>
       </c>
       <c r="E13" s="5">
         <v>0</v>
@@ -1480,19 +1661,20 @@
         <v>9</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="O13" s="1"/>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="11"/>
       <c r="B14" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="5">
@@ -1518,24 +1700,25 @@
         <v>9</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="11"/>
       <c r="B15" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="E15" s="5">
         <v>0</v>
@@ -1560,22 +1743,23 @@
         <v>9</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="O15" s="1"/>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="12"/>
       <c r="B16" s="2" t="s">
         <v>26</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E16" s="5">
         <v>0</v>
@@ -1600,22 +1784,23 @@
         <v>6</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="O16" s="1"/>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="11"/>
       <c r="B17" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="E17" s="5">
         <v>0</v>
@@ -1640,22 +1825,23 @@
         <v>9</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="O17" s="1"/>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="11"/>
       <c r="B18" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="E18" s="5">
         <v>-2</v>
@@ -1683,19 +1869,20 @@
         <v>11</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="O18" s="1"/>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="17"/>
       <c r="B19" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="E19" s="5">
         <v>-2</v>
@@ -1720,22 +1907,23 @@
         <v>9</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="O19" s="1"/>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="12"/>
       <c r="B20" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="E20" s="5">
         <v>0</v>
@@ -1760,22 +1948,23 @@
         <v>9</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="O20" s="1"/>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="11"/>
       <c r="B21" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="E21" s="5">
         <v>0</v>
@@ -1800,22 +1989,23 @@
         <v>9</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="O21" s="1"/>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="11"/>
       <c r="B22" s="2" t="s">
         <v>14</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="E22" s="5">
         <v>0</v>
@@ -1840,22 +2030,23 @@
         <v>9</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="O22" s="1"/>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="11"/>
       <c r="B23" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E23" s="5">
         <v>-2</v>
@@ -1880,22 +2071,23 @@
         <v>9</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="O23" s="1"/>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="11"/>
       <c r="B24" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="E24" s="5">
         <v>-4</v>
@@ -1920,105 +2112,108 @@
         <v>9</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="O24" s="1"/>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="11"/>
       <c r="B25" s="2" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E25" s="5">
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="F25" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G25" s="5">
         <v>0</v>
       </c>
       <c r="H25" s="5">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="I25" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J25" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K25" s="1"/>
       <c r="L25" s="4">
         <v>9</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>116</v>
+        <v>99</v>
       </c>
       <c r="N25" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="O25" s="1"/>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="11"/>
       <c r="B26" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E26" s="5">
+        <v>4</v>
+      </c>
+      <c r="F26" s="5">
+        <v>0</v>
+      </c>
+      <c r="G26" s="5">
+        <v>0</v>
+      </c>
+      <c r="H26" s="5">
         <v>-2</v>
       </c>
-      <c r="F26" s="5">
-        <v>2</v>
-      </c>
-      <c r="G26" s="5">
-        <v>0</v>
-      </c>
-      <c r="H26" s="5">
-        <v>0</v>
-      </c>
       <c r="I26" s="5">
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="J26" s="5">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="K26" s="1"/>
       <c r="L26" s="4">
         <v>9</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>106</v>
+        <v>85</v>
       </c>
       <c r="N26" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="O26" s="1"/>
     </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="11"/>
       <c r="B27" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="E27" s="5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F27" s="5">
         <v>0</v>
@@ -2027,198 +2222,203 @@
         <v>0</v>
       </c>
       <c r="H27" s="5">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="I27" s="5">
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="J27" s="5">
         <v>-2</v>
       </c>
       <c r="K27" s="1"/>
       <c r="L27" s="4">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="N27" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="O27" s="1"/>
     </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="11"/>
       <c r="B28" s="2" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="E28" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F28" s="5">
         <v>0</v>
       </c>
       <c r="G28" s="5">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="H28" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I28" s="5">
         <v>2</v>
       </c>
       <c r="J28" s="5">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="K28" s="1"/>
       <c r="L28" s="4">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>107</v>
+        <v>86</v>
       </c>
       <c r="N28" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="O28" s="1"/>
     </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="11"/>
       <c r="B29" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E29" s="5">
         <v>0</v>
       </c>
       <c r="F29" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G29" s="5">
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="H29" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I29" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J29" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K29" s="1"/>
       <c r="L29" s="4">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="N29" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="O29" s="1"/>
     </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="11"/>
       <c r="B30" s="2" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="E30" s="5">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="F30" s="5">
         <v>2</v>
       </c>
       <c r="G30" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H30" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I30" s="5">
         <v>0</v>
       </c>
       <c r="J30" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K30" s="1"/>
       <c r="L30" s="4">
         <v>6</v>
       </c>
       <c r="M30" s="2" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="N30" s="2" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="O30" s="1"/>
     </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="11"/>
       <c r="B31" s="2" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
       <c r="E31" s="5">
+        <v>2</v>
+      </c>
+      <c r="F31" s="5">
+        <v>0</v>
+      </c>
+      <c r="G31" s="5">
+        <v>0</v>
+      </c>
+      <c r="H31" s="5">
         <v>-2</v>
       </c>
-      <c r="F31" s="5">
-        <v>2</v>
-      </c>
-      <c r="G31" s="5">
-        <v>0</v>
-      </c>
-      <c r="H31" s="5">
-        <v>2</v>
-      </c>
       <c r="I31" s="5">
         <v>0</v>
       </c>
       <c r="J31" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K31" s="1"/>
       <c r="L31" s="4">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="M31" s="2" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="N31" s="2" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="O31" s="1"/>
     </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="16"/>
       <c r="B32" s="2" t="s">
         <v>32</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="E32" s="5">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="F32" s="5">
         <v>2</v>
@@ -2230,81 +2430,83 @@
         <v>0</v>
       </c>
       <c r="I32" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J32" s="5">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="K32" s="1"/>
       <c r="L32" s="4">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="M32" s="2" t="s">
-        <v>32</v>
+        <v>111</v>
       </c>
       <c r="N32" s="2" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="O32" s="1"/>
     </row>
-    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33" s="11"/>
       <c r="B33" s="2" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="E33" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F33" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G33" s="5">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="H33" s="5">
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="I33" s="5">
         <v>0</v>
       </c>
       <c r="J33" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K33" s="1"/>
       <c r="L33" s="4">
         <v>9</v>
       </c>
       <c r="M33" s="2" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="N33" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="O33" s="1"/>
     </row>
-    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34" s="16"/>
       <c r="B34" s="2" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="E34" s="5">
+        <v>0</v>
+      </c>
+      <c r="F34" s="5">
+        <v>2</v>
+      </c>
+      <c r="G34" s="5">
         <v>-2</v>
-      </c>
-      <c r="F34" s="5">
-        <v>2</v>
-      </c>
-      <c r="G34" s="5">
-        <v>0</v>
       </c>
       <c r="H34" s="5">
         <v>0</v>
@@ -2317,25 +2519,26 @@
       </c>
       <c r="K34" s="1"/>
       <c r="L34" s="4">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="M34" s="2" t="s">
-        <v>118</v>
+        <v>87</v>
       </c>
       <c r="N34" s="2" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="O34" s="1"/>
     </row>
-    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" s="15"/>
       <c r="B35" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E35" s="5">
         <v>0</v>
@@ -2344,38 +2547,39 @@
         <v>2</v>
       </c>
       <c r="G35" s="5">
+        <v>0</v>
+      </c>
+      <c r="H35" s="5">
+        <v>2</v>
+      </c>
+      <c r="I35" s="5">
+        <v>0</v>
+      </c>
+      <c r="J35" s="5">
         <v>-2</v>
-      </c>
-      <c r="H35" s="5">
-        <v>2</v>
-      </c>
-      <c r="I35" s="5">
-        <v>0</v>
-      </c>
-      <c r="J35" s="5">
-        <v>0</v>
       </c>
       <c r="K35" s="1"/>
       <c r="L35" s="4">
         <v>9</v>
       </c>
       <c r="M35" s="2" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="N35" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="O35" s="1"/>
     </row>
-    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A36" s="11"/>
       <c r="B36" s="2" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="E36" s="5">
         <v>0</v>
@@ -2384,38 +2588,39 @@
         <v>2</v>
       </c>
       <c r="G36" s="5">
+        <v>0</v>
+      </c>
+      <c r="H36" s="5">
+        <v>0</v>
+      </c>
+      <c r="I36" s="5">
+        <v>2</v>
+      </c>
+      <c r="J36" s="5">
         <v>-2</v>
-      </c>
-      <c r="H36" s="5">
-        <v>0</v>
-      </c>
-      <c r="I36" s="5">
-        <v>2</v>
-      </c>
-      <c r="J36" s="5">
-        <v>0</v>
       </c>
       <c r="K36" s="1"/>
       <c r="L36" s="4">
         <v>9</v>
       </c>
       <c r="M36" s="2" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="N36" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="O36" s="1"/>
     </row>
-    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A37" s="11"/>
       <c r="B37" s="2" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>69</v>
+        <v>44</v>
       </c>
       <c r="E37" s="5">
         <v>0</v>
@@ -2427,145 +2632,595 @@
         <v>0</v>
       </c>
       <c r="H37" s="5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I37" s="5">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="J37" s="5">
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="K37" s="1"/>
       <c r="L37" s="4">
         <v>9</v>
       </c>
       <c r="M37" s="2" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="N37" s="2" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="O37" s="1"/>
     </row>
-    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B38" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="E38" s="5">
-        <v>0</v>
-      </c>
-      <c r="F38" s="5">
-        <v>2</v>
-      </c>
-      <c r="G38" s="5">
-        <v>0</v>
-      </c>
-      <c r="H38" s="5">
-        <v>0</v>
-      </c>
-      <c r="I38" s="5">
-        <v>2</v>
-      </c>
-      <c r="J38" s="5">
-        <v>-2</v>
-      </c>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A38" s="11"/>
+      <c r="B38" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+      <c r="I38" s="9"/>
+      <c r="J38" s="9"/>
       <c r="K38" s="1"/>
-      <c r="L38" s="4">
-        <v>9</v>
-      </c>
-      <c r="M38" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="N38" s="2" t="s">
-        <v>86</v>
-      </c>
+      <c r="L38" s="10"/>
+      <c r="M38" s="1"/>
+      <c r="N38" s="1"/>
       <c r="O38" s="1"/>
     </row>
-    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B39" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="E39" s="5">
-        <v>0</v>
-      </c>
-      <c r="F39" s="5">
-        <v>2</v>
-      </c>
-      <c r="G39" s="5">
-        <v>0</v>
-      </c>
-      <c r="H39" s="5">
-        <v>0</v>
-      </c>
-      <c r="I39" s="5">
-        <v>-2</v>
-      </c>
-      <c r="J39" s="5">
-        <v>2</v>
-      </c>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A39" s="11"/>
+      <c r="B39" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="9"/>
+      <c r="H39" s="9"/>
+      <c r="I39" s="9"/>
+      <c r="J39" s="9"/>
       <c r="K39" s="1"/>
-      <c r="L39" s="4">
-        <v>9</v>
-      </c>
-      <c r="M39" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="N39" s="2" t="s">
-        <v>86</v>
-      </c>
+      <c r="L39" s="10"/>
+      <c r="M39" s="1"/>
+      <c r="N39" s="1"/>
       <c r="O39" s="1"/>
     </row>
-    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B40" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D40" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E40" s="5">
-        <v>0</v>
-      </c>
-      <c r="F40" s="5">
-        <v>2</v>
-      </c>
-      <c r="G40" s="5">
-        <v>0</v>
-      </c>
-      <c r="H40" s="5">
-        <v>2</v>
-      </c>
-      <c r="I40" s="5">
-        <v>-2</v>
-      </c>
-      <c r="J40" s="5">
-        <v>0</v>
-      </c>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A40" s="17"/>
+      <c r="B40" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
+      <c r="I40" s="9"/>
+      <c r="J40" s="9"/>
       <c r="K40" s="1"/>
-      <c r="L40" s="4">
-        <v>6</v>
-      </c>
-      <c r="M40" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="N40" s="2" t="s">
-        <v>87</v>
-      </c>
+      <c r="L40" s="10"/>
+      <c r="M40" s="1"/>
+      <c r="N40" s="1"/>
       <c r="O40" s="1"/>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A41" s="12"/>
+      <c r="B41" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9"/>
+      <c r="H41" s="9"/>
+      <c r="I41" s="9"/>
+      <c r="J41" s="9"/>
+      <c r="K41" s="1"/>
+      <c r="L41" s="10"/>
+      <c r="M41" s="1"/>
+      <c r="N41" s="1"/>
+      <c r="O41" s="1"/>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A42" s="17"/>
+      <c r="B42" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="9"/>
+      <c r="H42" s="9"/>
+      <c r="I42" s="9"/>
+      <c r="J42" s="9"/>
+      <c r="K42" s="1"/>
+      <c r="L42" s="10"/>
+      <c r="M42" s="1"/>
+      <c r="N42" s="1"/>
+      <c r="O42" s="1"/>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A43" s="11"/>
+      <c r="B43" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
+      <c r="G43" s="9"/>
+      <c r="H43" s="9"/>
+      <c r="I43" s="9"/>
+      <c r="J43" s="9"/>
+      <c r="K43" s="1"/>
+      <c r="L43" s="10"/>
+      <c r="M43" s="1"/>
+      <c r="N43" s="1"/>
+      <c r="O43" s="1"/>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A44" s="11"/>
+      <c r="B44" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="9"/>
+      <c r="G44" s="9"/>
+      <c r="H44" s="9"/>
+      <c r="I44" s="9"/>
+      <c r="J44" s="9"/>
+      <c r="K44" s="1"/>
+      <c r="L44" s="10"/>
+      <c r="M44" s="1"/>
+      <c r="N44" s="1"/>
+      <c r="O44" s="1"/>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A45" s="11"/>
+      <c r="B45" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="9"/>
+      <c r="G45" s="9"/>
+      <c r="H45" s="9"/>
+      <c r="I45" s="9"/>
+      <c r="J45" s="9"/>
+      <c r="K45" s="1"/>
+      <c r="L45" s="10"/>
+      <c r="M45" s="1"/>
+      <c r="N45" s="1"/>
+      <c r="O45" s="1"/>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A46" s="11"/>
+      <c r="B46" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="9"/>
+      <c r="G46" s="9"/>
+      <c r="H46" s="9"/>
+      <c r="I46" s="9"/>
+      <c r="J46" s="9"/>
+      <c r="K46" s="1"/>
+      <c r="L46" s="10"/>
+      <c r="M46" s="1"/>
+      <c r="N46" s="1"/>
+      <c r="O46" s="1"/>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A47" s="17"/>
+      <c r="B47" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="9"/>
+      <c r="G47" s="9"/>
+      <c r="H47" s="9"/>
+      <c r="I47" s="9"/>
+      <c r="J47" s="9"/>
+      <c r="K47" s="1"/>
+      <c r="L47" s="10"/>
+      <c r="M47" s="1"/>
+      <c r="N47" s="1"/>
+      <c r="O47" s="1"/>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A48" s="12"/>
+      <c r="B48" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="9"/>
+      <c r="G48" s="9"/>
+      <c r="H48" s="9"/>
+      <c r="I48" s="9"/>
+      <c r="J48" s="9"/>
+      <c r="K48" s="1"/>
+      <c r="L48" s="10"/>
+      <c r="M48" s="1"/>
+      <c r="N48" s="1"/>
+      <c r="O48" s="1"/>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A49" s="11"/>
+      <c r="B49" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="9"/>
+      <c r="G49" s="9"/>
+      <c r="H49" s="9"/>
+      <c r="I49" s="9"/>
+      <c r="J49" s="9"/>
+      <c r="K49" s="1"/>
+      <c r="L49" s="10"/>
+      <c r="M49" s="1"/>
+      <c r="N49" s="1"/>
+      <c r="O49" s="1"/>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A50" s="12"/>
+      <c r="B50" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9"/>
+      <c r="G50" s="9"/>
+      <c r="H50" s="9"/>
+      <c r="I50" s="9"/>
+      <c r="J50" s="9"/>
+      <c r="K50" s="1"/>
+      <c r="L50" s="10"/>
+      <c r="M50" s="1"/>
+      <c r="N50" s="1"/>
+      <c r="O50" s="1"/>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A51" s="11"/>
+      <c r="B51" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="9"/>
+      <c r="G51" s="9"/>
+      <c r="H51" s="9"/>
+      <c r="I51" s="9"/>
+      <c r="J51" s="9"/>
+      <c r="K51" s="1"/>
+      <c r="L51" s="10"/>
+      <c r="M51" s="1"/>
+      <c r="N51" s="1"/>
+      <c r="O51" s="1"/>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A52" s="13"/>
+      <c r="B52" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+      <c r="E52" s="9"/>
+      <c r="F52" s="9"/>
+      <c r="G52" s="9"/>
+      <c r="H52" s="9"/>
+      <c r="I52" s="9"/>
+      <c r="J52" s="9"/>
+      <c r="K52" s="1"/>
+      <c r="L52" s="10"/>
+      <c r="M52" s="1"/>
+      <c r="N52" s="1"/>
+      <c r="O52" s="1"/>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A53" s="17"/>
+      <c r="B53" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="9"/>
+      <c r="F53" s="9"/>
+      <c r="G53" s="9"/>
+      <c r="H53" s="9"/>
+      <c r="I53" s="9"/>
+      <c r="J53" s="9"/>
+      <c r="K53" s="1"/>
+      <c r="L53" s="10"/>
+      <c r="M53" s="1"/>
+      <c r="N53" s="1"/>
+      <c r="O53" s="1"/>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A54" s="13"/>
+      <c r="B54" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="9"/>
+      <c r="F54" s="9"/>
+      <c r="G54" s="9"/>
+      <c r="H54" s="9"/>
+      <c r="I54" s="9"/>
+      <c r="J54" s="9"/>
+      <c r="K54" s="1"/>
+      <c r="L54" s="10"/>
+      <c r="M54" s="1"/>
+      <c r="N54" s="1"/>
+      <c r="O54" s="1"/>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A55" s="11"/>
+      <c r="B55" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="9"/>
+      <c r="F55" s="9"/>
+      <c r="G55" s="9"/>
+      <c r="H55" s="9"/>
+      <c r="I55" s="9"/>
+      <c r="J55" s="9"/>
+      <c r="K55" s="1"/>
+      <c r="L55" s="10"/>
+      <c r="M55" s="1"/>
+      <c r="N55" s="1"/>
+      <c r="O55" s="1"/>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A56" s="12"/>
+      <c r="B56" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="9"/>
+      <c r="F56" s="9"/>
+      <c r="G56" s="9"/>
+      <c r="H56" s="9"/>
+      <c r="I56" s="9"/>
+      <c r="J56" s="9"/>
+      <c r="K56" s="1"/>
+      <c r="L56" s="10"/>
+      <c r="M56" s="1"/>
+      <c r="N56" s="1"/>
+      <c r="O56" s="1"/>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A57" s="11"/>
+      <c r="B57" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="9"/>
+      <c r="F57" s="9"/>
+      <c r="G57" s="9"/>
+      <c r="H57" s="9"/>
+      <c r="I57" s="9"/>
+      <c r="J57" s="9"/>
+      <c r="K57" s="1"/>
+      <c r="L57" s="10"/>
+      <c r="M57" s="1"/>
+      <c r="N57" s="1"/>
+      <c r="O57" s="1"/>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A58" s="11"/>
+      <c r="B58" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="9"/>
+      <c r="F58" s="9"/>
+      <c r="G58" s="9"/>
+      <c r="H58" s="9"/>
+      <c r="I58" s="9"/>
+      <c r="J58" s="9"/>
+      <c r="K58" s="1"/>
+      <c r="L58" s="10"/>
+      <c r="M58" s="1"/>
+      <c r="N58" s="1"/>
+      <c r="O58" s="1"/>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A59" s="11"/>
+      <c r="B59" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="9"/>
+      <c r="F59" s="9"/>
+      <c r="G59" s="9"/>
+      <c r="H59" s="9"/>
+      <c r="I59" s="9"/>
+      <c r="J59" s="9"/>
+      <c r="K59" s="1"/>
+      <c r="L59" s="10"/>
+      <c r="M59" s="1"/>
+      <c r="N59" s="1"/>
+      <c r="O59" s="1"/>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A60" s="13"/>
+      <c r="B60" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="9"/>
+      <c r="F60" s="9"/>
+      <c r="G60" s="9"/>
+      <c r="H60" s="9"/>
+      <c r="I60" s="9"/>
+      <c r="J60" s="9"/>
+      <c r="K60" s="1"/>
+      <c r="L60" s="10"/>
+      <c r="M60" s="1"/>
+      <c r="N60" s="1"/>
+      <c r="O60" s="1"/>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A61" s="13"/>
+      <c r="B61" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="9"/>
+      <c r="F61" s="9"/>
+      <c r="G61" s="9"/>
+      <c r="H61" s="9"/>
+      <c r="I61" s="9"/>
+      <c r="J61" s="9"/>
+      <c r="K61" s="1"/>
+      <c r="L61" s="10"/>
+      <c r="M61" s="1"/>
+      <c r="N61" s="1"/>
+      <c r="O61" s="1"/>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A62" s="12"/>
+      <c r="B62" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C62" s="1"/>
+      <c r="D62" s="1"/>
+      <c r="E62" s="9"/>
+      <c r="F62" s="9"/>
+      <c r="G62" s="9"/>
+      <c r="H62" s="9"/>
+      <c r="I62" s="9"/>
+      <c r="J62" s="9"/>
+      <c r="K62" s="1"/>
+      <c r="L62" s="10"/>
+      <c r="M62" s="1"/>
+      <c r="N62" s="1"/>
+      <c r="O62" s="1"/>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A63" s="11"/>
+      <c r="B63" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="9"/>
+      <c r="F63" s="9"/>
+      <c r="G63" s="9"/>
+      <c r="H63" s="9"/>
+      <c r="I63" s="9"/>
+      <c r="J63" s="9"/>
+      <c r="K63" s="1"/>
+      <c r="L63" s="10"/>
+      <c r="M63" s="1"/>
+      <c r="N63" s="1"/>
+      <c r="O63" s="1"/>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A64" s="12"/>
+      <c r="B64" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C64" s="1"/>
+      <c r="D64" s="1"/>
+      <c r="E64" s="9"/>
+      <c r="F64" s="9"/>
+      <c r="G64" s="9"/>
+      <c r="H64" s="9"/>
+      <c r="I64" s="9"/>
+      <c r="J64" s="9"/>
+      <c r="K64" s="1"/>
+      <c r="L64" s="10"/>
+      <c r="M64" s="1"/>
+      <c r="N64" s="1"/>
+      <c r="O64" s="1"/>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A65" s="13"/>
+      <c r="B65" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C65" s="1"/>
+      <c r="D65" s="1"/>
+      <c r="E65" s="9"/>
+      <c r="F65" s="9"/>
+      <c r="G65" s="9"/>
+      <c r="H65" s="9"/>
+      <c r="I65" s="9"/>
+      <c r="J65" s="9"/>
+      <c r="K65" s="1"/>
+      <c r="L65" s="10"/>
+      <c r="M65" s="1"/>
+      <c r="N65" s="1"/>
+      <c r="O65" s="1"/>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A66" s="13"/>
+      <c r="B66" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C66" s="1"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="9"/>
+      <c r="F66" s="9"/>
+      <c r="G66" s="9"/>
+      <c r="H66" s="9"/>
+      <c r="I66" s="9"/>
+      <c r="J66" s="9"/>
+      <c r="K66" s="1"/>
+      <c r="L66" s="10"/>
+      <c r="M66" s="1"/>
+      <c r="N66" s="1"/>
+      <c r="O66" s="1"/>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A67" s="17"/>
+      <c r="B67" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C67" s="1"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="9"/>
+      <c r="F67" s="9"/>
+      <c r="G67" s="9"/>
+      <c r="H67" s="9"/>
+      <c r="I67" s="9"/>
+      <c r="J67" s="9"/>
+      <c r="K67" s="1"/>
+      <c r="L67" s="10"/>
+      <c r="M67" s="1"/>
+      <c r="N67" s="1"/>
+      <c r="O67" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>